<commit_message>
refactor for settings change done
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD726177-17F6-5648-8A3A-C1E228A15829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812B415D-EC0D-1B4A-9762-6E466019E934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="-24840" windowWidth="21600" windowHeight="37940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>url</t>
   </si>
@@ -110,12 +110,6 @@
     <t>t2-Busi-U</t>
   </si>
   <si>
-    <t>https://order-tst.nonprod.jbhunt.com/order/automationrules</t>
-  </si>
-  <si>
-    <t>jisavr3</t>
-  </si>
-  <si>
     <t>createdBy</t>
   </si>
   <si>
@@ -140,19 +134,22 @@
     <t>t2-Cus</t>
   </si>
   <si>
-    <t>USFOOD</t>
-  </si>
-  <si>
-    <t>KIMBERLY</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>https://order-tst-prof2.nonprod.jbhunt.com/order/automationrules</t>
+  </si>
+  <si>
+    <t>99CENTS</t>
+  </si>
+  <si>
+    <t>JISQHX3</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -319,8 +316,9 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -748,7 +746,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -757,6 +754,7 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -806,17 +804,23 @@
   <dxfs count="59">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -840,21 +844,100 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1277,22 +1360,40 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1334,7 +1435,101 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1375,6 +1570,454 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1397,8 +2040,186 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1421,232 +2242,26 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1655,650 +2270,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2314,25 +2285,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:D2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="58" headerRowBorderDxfId="39" tableBorderDxfId="40" totalsRowBorderDxfId="38">
-  <autoFilter ref="A1:D2" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:D3" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+  <autoFilter ref="A1:D3" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="37" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="57" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:D2" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2340,17 +2311,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="56" headerRowBorderDxfId="54" tableBorderDxfId="55" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L2" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="A1:L2" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2366,39 +2337,39 @@
     <filterColumn colId="11" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:B2" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:B2" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:B2" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="fileName" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="tabName" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="fileName" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="tabName" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:M2" xr:uid="{B5B17CF2-012E-764F-A3B1-44C7505ECF30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2415,19 +2386,19 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2730,15 +2701,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
@@ -2746,28 +2717,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>28</v>
+      <c r="A2" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2785,7 +2762,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2798,17 +2775,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2816,7 +2793,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -2838,61 +2815,61 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="10.5" style="2" customWidth="1"/>
     <col min="13" max="16384" width="14.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>34</v>
+      <c r="K1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -2919,10 +2896,10 @@
         <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2937,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F814824A-BE6E-4AC5-90CF-CA8866E1DFA9}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2948,40 +2925,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3007,44 +2984,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>34</v>
+      <c r="L1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
append missing code before save rule
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD306F3A-DD81-7C45-B98F-626AACAA39F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC18A51-2964-8846-A5FE-457C9B34E686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-24840" windowWidth="21600" windowHeight="37940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>url</t>
   </si>
@@ -134,19 +134,22 @@
     <t>username</t>
   </si>
   <si>
-    <t>99CENTS</t>
-  </si>
-  <si>
-    <t>JISQHX3</t>
-  </si>
-  <si>
     <t>https://order-tst.nonprod.jbhunt.com/order/automationrules</t>
   </si>
   <si>
-    <t>JCPENNEY</t>
-  </si>
-  <si>
-    <t>simpleton</t>
+    <t>ARCONICTP</t>
+  </si>
+  <si>
+    <t>ARCONICTP_HJBT 06.15.2020</t>
+  </si>
+  <si>
+    <t>ARCONICTP_HJBB 06.15.2020</t>
+  </si>
+  <si>
+    <t>simpletonTest</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -848,9 +851,7 @@
         <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -863,356 +864,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -1221,40 +872,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1342,7 +975,9 @@
         <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1355,6 +990,356 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -1376,6 +1361,24 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2319,8 +2322,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L2" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="A1:L2" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:L3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="A1:L3" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2353,21 +2356,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:B2" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:B2" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B2" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="fileName" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="tabName" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="fileName" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="tabName" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:M2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:M2" xr:uid="{B5B17CF2-012E-764F-A3B1-44C7505ECF30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2384,19 +2387,19 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2701,7 +2704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2730,7 +2733,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -2788,11 +2791,9 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4">
         <v>3</v>
       </c>
@@ -2810,16 +2811,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ED05CD-C67D-D046-9F19-D31D60A54D78}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="10.5" style="2" customWidth="1"/>
     <col min="13" max="16384" width="14.83203125" style="2"/>
   </cols>
@@ -2864,7 +2865,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>39</v>
@@ -2897,6 +2898,44 @@
         <v>32</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2912,14 +2951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F814824A-BE6E-4AC5-90CF-CA8866E1DFA9}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2942,10 +2982,10 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2971,7 +3011,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="G1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
last commit was inside subfolder test by accident, commit the rest
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A97AED3-F0DB-BD40-98A5-C223E309F7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E61167-A169-0644-983D-A6D544A66364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>url</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>TJMAXnew 2</t>
+  </si>
+  <si>
+    <t>TPCCOV</t>
+  </si>
+  <si>
+    <t>COCHDQ</t>
+  </si>
+  <si>
+    <t>EXSP6</t>
+  </si>
+  <si>
+    <t>BROK</t>
   </si>
 </sst>
 </file>
@@ -2772,8 +2784,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E5" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="A1:E5" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="A1:E6" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2792,8 +2804,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H5" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A1:H5" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H6" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:H6" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3154,8 +3166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3494,10 +3506,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3539,7 +3551,9 @@
       <c r="D2" s="17">
         <v>2</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="26" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
@@ -3563,7 +3577,9 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -3581,6 +3597,21 @@
       <c r="E5" s="5" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3595,10 +3626,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3652,7 +3683,9 @@
         <v>48</v>
       </c>
       <c r="G2" s="22"/>
-      <c r="H2" s="26"/>
+      <c r="H2" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -3672,7 +3705,9 @@
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="H3" s="23" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
@@ -3708,7 +3743,29 @@
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="20"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3725,7 +3782,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new login page, backward compatible
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E61167-A169-0644-983D-A6D544A66364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5272615-8AA7-944E-9947-0FC329FE6BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
   <si>
     <t>url</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>BROK</t>
+  </si>
+  <si>
+    <t>newLoginPage</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -929,6 +932,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -975,7 +979,51 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2534,18 +2582,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2728,27 +2764,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:E3" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
-  <autoFilter ref="A1:E3" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:F3" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+  <autoFilter ref="A1:F3" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="63" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{53246AB4-3995-C043-A4E0-8E6B3CA6C3E2}" name="SKIP" dataDxfId="59"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="64" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{D5B508CA-B917-0E4B-A808-A4A4DB67A285}" name="newLoginPage" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{82D8753C-3297-1C4F-8965-5A98C6FBEDE7}" name="SKIP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M6" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M6" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="A1:M6" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2765,26 +2803,26 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{D6E44FEE-839E-8D45-BE21-BF61FDD7208F}" name="SKIP" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{D6E44FEE-839E-8D45-BE21-BF61FDD7208F}" name="SKIP" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E6" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="A1:E6" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2793,18 +2831,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{0624CFA4-F6C8-D846-9648-BFA84E5E19BD}" name="SKIP" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{0624CFA4-F6C8-D846-9648-BFA84E5E19BD}" name="SKIP" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H6" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H6" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A1:H6" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2816,21 +2854,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="Trading Partner" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="SCAC" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{A1748E27-D6A4-EE42-86D0-6C6739CDB0DC}" name="BTC" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6F092B60-79E4-164F-BD1C-798DCF2D379B}" name="Corp Acct" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{D4701DF2-1CFF-7147-9AE0-075DE4FC5844}" name="BU" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{40A4A830-9458-204F-B09B-879E27281E1A}" name="SO" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{F56EDCFC-C0D1-BA47-A3C6-E646104EFFC4}" name="Fleet" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{6CC83267-4862-7D4E-9AD1-52EF248B010A}" name="SKIP" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="Trading Partner" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="SCAC" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{A1748E27-D6A4-EE42-86D0-6C6739CDB0DC}" name="BTC" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{6F092B60-79E4-164F-BD1C-798DCF2D379B}" name="Corp Acct" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{D4701DF2-1CFF-7147-9AE0-075DE4FC5844}" name="BU" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{40A4A830-9458-204F-B09B-879E27281E1A}" name="SO" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{F56EDCFC-C0D1-BA47-A3C6-E646104EFFC4}" name="Fleet" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{6CC83267-4862-7D4E-9AD1-52EF248B010A}" name="SKIP" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:N3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5FBCBAA8-0386-4B4F-8826-46FD915F103C}" name="Table11" displayName="Table11" ref="A1:N3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:N3" xr:uid="{B5B17CF2-012E-764F-A3B1-44C7505ECF30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2848,20 +2886,20 @@
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{C862A3A6-36B4-FF41-8233-ED3AD300F387}" name="SKIP" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D5F5E6A1-2B72-7F41-8016-996CDA62DE12}" name="missingCodeFileName" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{741294D1-F604-CC4A-917D-9BFEC40EA974}" name="ruleDataFileName" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{D90BCCCC-60DE-E140-8EA8-9C68920FC3E3}" name="newFileName" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0F1C21AD-5DCA-2445-AAD5-65278C3DA304}" name="t1bt" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{831B61E6-9836-7E43-AD5B-689EC75DC91F}" name="t2bt" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{967D2A40-3B01-A44A-8EC4-DE08B2A7DB9C}" name="t1bu" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{1F9B7FB5-ED4F-F049-9579-548D513A89A5}" name="t2bu" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{3894DDE8-0A5C-C346-BE15-6A8842257ABE}" name="t1so" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{488C3AE5-D292-EE4C-AAB0-F85A3C34E5BB}" name="t2so" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{5E123C06-E039-CB4F-886C-B626069D549C}" name="t1fl" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{3B39AD1D-E4D3-B54A-86CE-68BC61D6D409}" name="t2fl" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{724A8853-215F-E941-B4A2-B96EC61D4648}" name="t1cu" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{908C0810-E77F-474C-8C5D-79C69A3CE84C}" name="t2cu" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{C862A3A6-36B4-FF41-8233-ED3AD300F387}" name="SKIP" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3164,10 +3202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3176,11 +3214,12 @@
     <col min="2" max="2" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="55.1640625" style="2"/>
+    <col min="5" max="5" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="55.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3193,11 +3232,14 @@
       <c r="D1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>53</v>
       </c>
@@ -3206,11 +3248,12 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="2" t="b">
+      <c r="E2" s="17" t="b">
         <v>1</v>
       </c>
+      <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>49</v>
       </c>
@@ -3219,6 +3262,8 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3237,7 +3282,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,7 +3554,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3602,9 +3647,7 @@
       <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4">
         <v>3</v>
       </c>
@@ -3629,7 +3672,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3783,7 +3826,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
not clickable exception, so acronym bug
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0700135D-C6C0-EA41-BCA0-41E434940A89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4B0D75-C7FB-C747-A388-246343F4AF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="65">
   <si>
     <t>url</t>
   </si>
@@ -164,15 +164,9 @@
     <t>ARCONIC</t>
   </si>
   <si>
-    <t>ALPI37</t>
-  </si>
-  <si>
     <t>ICS</t>
   </si>
   <si>
-    <t>Brok</t>
-  </si>
-  <si>
     <t>https://order-tst-prof2.nonprod.jbhunt.com/order/automationrules</t>
   </si>
   <si>
@@ -188,24 +182,9 @@
     <t>https://order-tst.nonprod.jbhunt.com/order/automationrules</t>
   </si>
   <si>
-    <t>ALENDIST</t>
-  </si>
-  <si>
     <t>HJBT</t>
   </si>
   <si>
-    <t>BARCH4</t>
-  </si>
-  <si>
-    <t>JBT</t>
-  </si>
-  <si>
-    <t>OTR</t>
-  </si>
-  <si>
-    <t>CBCAAB</t>
-  </si>
-  <si>
     <t>ARCONIC_HJBBnewsorting 6.15.20</t>
   </si>
   <si>
@@ -233,25 +212,13 @@
     <t>TPCCOV</t>
   </si>
   <si>
-    <t>COCHDQ</t>
-  </si>
-  <si>
-    <t>EXSP6</t>
-  </si>
-  <si>
-    <t>BROK</t>
-  </si>
-  <si>
     <t>newLoginPage</t>
   </si>
   <si>
-    <t>CHRMAUSER</t>
-  </si>
-  <si>
-    <t>CHRMAUSER_HJBB</t>
-  </si>
-  <si>
-    <t>t2-btc-2</t>
+    <t>Flatbed</t>
+  </si>
+  <si>
+    <t>HJBB</t>
   </si>
 </sst>
 </file>
@@ -2655,8 +2622,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M7" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
-  <autoFilter ref="A1:M7" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M6" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+  <autoFilter ref="A1:M6" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2711,8 +2678,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A1:H6" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H3" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:H3" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3074,7 +3041,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3102,15 +3069,15 @@
         <v>33</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="10">
         <v>2</v>
@@ -3124,7 +3091,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="10">
         <v>3</v>
@@ -3148,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ED05CD-C67D-D046-9F19-D31D60A54D78}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3200,7 +3167,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3240,9 +3207,7 @@
       <c r="L2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="19" t="b">
-        <v>1</v>
-      </c>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -3290,7 +3255,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -3331,7 +3296,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -3369,10 +3334,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -3405,27 +3370,6 @@
         <v>32</v>
       </c>
       <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -3444,7 +3388,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3470,7 +3414,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3478,7 +3422,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="7">
         <v>3</v>
@@ -3486,9 +3430,7 @@
       <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -3507,7 +3449,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -3518,10 +3460,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -3535,7 +3477,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10">
@@ -3544,7 +3486,9 @@
       <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3559,10 +3503,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3595,7 +3539,7 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
@@ -3603,104 +3547,40 @@
       <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
+      <c r="B3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3717,7 +3597,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3770,7 +3650,7 @@
         <v>29</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -3809,13 +3689,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
v1.13 check rule name when open configure new rule page; go back and retry when resultant action not appear
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4B0D75-C7FB-C747-A388-246343F4AF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7722CAD7-2376-A84A-994F-EFF5F1C4ECDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -3040,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3080,7 +3080,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11"/>
@@ -3597,7 +3597,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v1.13 handle exceptions for 3dots, resultant actions
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4B0D75-C7FB-C747-A388-246343F4AF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7722CAD7-2376-A84A-994F-EFF5F1C4ECDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -3040,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3080,7 +3080,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11"/>
@@ -3597,7 +3597,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
irrelevant data file changes
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE575E92-19D6-B84A-A804-65FBAB8930CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BC5454-703B-F14D-944F-C0CF2208B6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>url</t>
   </si>
@@ -131,15 +131,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>ARCONICTP</t>
-  </si>
-  <si>
-    <t>ARCONICTP_HJBT 06.15.2020</t>
-  </si>
-  <si>
-    <t>ARCONICTP_HJBB 06.15.2020</t>
-  </si>
-  <si>
     <t>Trading Partner</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>Fleet</t>
   </si>
   <si>
-    <t>ARCONIC</t>
-  </si>
-  <si>
     <t>ICS</t>
   </si>
   <si>
@@ -173,24 +161,12 @@
     <t>99CENTS</t>
   </si>
   <si>
-    <t>JISQHX3</t>
-  </si>
-  <si>
     <t>SKIP</t>
   </si>
   <si>
     <t>https://order-tst.nonprod.jbhunt.com/order/automationrules</t>
   </si>
   <si>
-    <t>HJBT</t>
-  </si>
-  <si>
-    <t>TRUCOIMG</t>
-  </si>
-  <si>
-    <t>jisavr3</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -203,16 +179,25 @@
     <t>TJMAXnew 2</t>
   </si>
   <si>
-    <t>TPCCOV</t>
-  </si>
-  <si>
     <t>newLoginPage</t>
   </si>
   <si>
-    <t>Flatbed</t>
-  </si>
-  <si>
     <t>HJBB</t>
+  </si>
+  <si>
+    <t>USFOOD</t>
+  </si>
+  <si>
+    <t>USCO61</t>
+  </si>
+  <si>
+    <t>KIKN5</t>
+  </si>
+  <si>
+    <t>HJBF</t>
+  </si>
+  <si>
+    <t>IRPI</t>
   </si>
 </sst>
 </file>
@@ -569,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -770,19 +755,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -852,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -865,20 +837,18 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2616,8 +2586,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M4" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
-  <autoFilter ref="A1:M4" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M3" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+  <autoFilter ref="A1:M3" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2652,8 +2622,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="A1:E6" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="A1:E3" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2672,8 +2642,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H3" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A1:H3" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H4" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:H4" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3034,7 +3004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9160359D-1B9E-284A-A763-80B627CB8CD3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3050,50 +3020,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>50</v>
+      <c r="E1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="10">
+        <v>46</v>
+      </c>
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="7" t="b">
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="10">
+        <v>43</v>
+      </c>
+      <c r="B3" s="9">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3109,10 +3079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ED05CD-C67D-D046-9F19-D31D60A54D78}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3124,164 +3094,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>50</v>
+      <c r="M1" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="19"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="10"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -3297,10 +3218,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3326,81 +3247,28 @@
         <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="7">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7">
-        <v>2</v>
-      </c>
-      <c r="E2" s="9"/>
+      <c r="A2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="10">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2</v>
-      </c>
-      <c r="E5" s="11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10">
-        <v>3</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2</v>
-      </c>
-      <c r="E6" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3415,10 +3283,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3430,69 +3298,85 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3522,116 +3406,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>50</v>
+      <c r="N1" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="16"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="15"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="A3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wdio5 tested on mac
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BC5454-703B-F14D-944F-C0CF2208B6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC2D979-761B-0443-8A6D-B1DA668A7CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -3081,7 +3081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ED05CD-C67D-D046-9F19-D31D60A54D78}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3221,7 +3221,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3257,9 +3257,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3268,7 +3266,9 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3285,8 +3285,8 @@
   </sheetPr>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3340,7 +3340,9 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="H2" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>

</xml_diff>

<commit_message>
maxTries and more retry
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/wdio6/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D907E-3DA1-374B-9CDA-720F38090791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD80870-28CA-9045-958C-101DEC250DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-18120" windowWidth="32680" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32900" yWindow="-20720" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>url</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>maxTries</t>
+  </si>
+  <si>
+    <t>HJBT</t>
+  </si>
+  <si>
+    <t>CAKE26</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -787,6 +793,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -833,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -862,6 +881,7 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2685,8 +2705,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H4" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A1:H4" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:H5" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3048,7 +3068,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3094,7 +3114,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
@@ -3132,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ED05CD-C67D-D046-9F19-D31D60A54D78}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3255,9 +3275,7 @@
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -3313,7 +3331,9 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="9"/>
+      <c r="M5" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -3332,7 +3352,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3368,7 +3388,9 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3377,9 +3399,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -3405,7 +3425,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
@@ -3470,37 +3490,61 @@
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
+    <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3517,7 +3561,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
convert rejected tender rule
</commit_message>
<xml_diff>
--- a/testdata/settings.xlsx
+++ b/testdata/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/wdio6/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD80870-28CA-9045-958C-101DEC250DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4864FDE8-93E6-A744-BA8C-A5EC45C298CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32900" yWindow="-20720" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="480" windowWidth="32680" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>url</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>CAKE26</t>
+  </si>
+  <si>
+    <t>Convert</t>
   </si>
 </sst>
 </file>
@@ -928,7 +931,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="73">
     <dxf>
       <font>
         <b val="0"/>
@@ -1449,6 +1452,36 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2625,7 +2658,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:G3" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9BB73794-A3F9-7840-AB43-105336261E1A}" name="Table79" displayName="Table79" ref="A1:G3" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="A1:G3" xr:uid="{D902FDEF-4A66-A249-8A9E-4C9476CD0585}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2636,20 +2669,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="66" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{15079ED4-DB26-F440-8FF0-CE818C6222C7}" name="maxTries" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{D5B508CA-B917-0E4B-A808-A4A4DB67A285}" name="newLoginPage" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{82D8753C-3297-1C4F-8965-5A98C6FBEDE7}" name="SKIP" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{40FB39B6-E6C9-E04C-8DC5-7B1EF7CF03CD}" name="url" dataDxfId="67" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{5E56D9C9-F570-1348-8269-D0AD78470E72}" name="delaySecond" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{15079ED4-DB26-F440-8FF0-CE818C6222C7}" name="maxTries" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{3FE4A58A-3B03-0F45-9086-BD7CC36ED774}" name="username" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{75FC3F85-123C-734E-A443-F78AC8D89B27}" name="password" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{D5B508CA-B917-0E4B-A808-A4A4DB67A285}" name="newLoginPage" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{82D8753C-3297-1C4F-8965-5A98C6FBEDE7}" name="SKIP" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F86466B9-99AA-EE42-9885-C66CE4CD392E}" name="Table9" displayName="Table9" ref="A1:M5" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="A1:M5" xr:uid="{115B8CD8-FD8D-6947-BFF4-7ABA0024CEC4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2666,26 +2699,26 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{D6E44FEE-839E-8D45-BE21-BF61FDD7208F}" name="SKIP" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{A02382E6-ADE3-A242-A202-192BBD90FAE7}" name="tradingPartner" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{74C6A343-DC32-3F4A-853C-100B3FC0E934}" name="fileName" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{A9E05B2F-FEED-424F-A6A7-6CB274608CBD}" name="t1bt" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{1872C4F0-C20C-AA44-8D7F-0C51AAC58F25}" name="t2bt" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{A576BB00-6B6F-AC42-8642-6CF7825FCABD}" name="t1bu" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{579AEECD-3CAD-794A-8DD3-324A8BD3E83C}" name="t2bu" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{75E0BC80-D6B0-C848-B965-EB9E71ED84FA}" name="t1so" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{D8392679-15A0-EA4D-A15D-8C3DD767BA31}" name="t2so" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{E46D819F-6CE5-1443-BC5D-6679813EE74A}" name="t1fl" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{BFD61505-7B07-6D48-8F42-187515D288C2}" name="t2fl" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{34C9D25B-DA7B-A745-9F3C-CD55679D0E9A}" name="t1cu" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{0AEE78C2-385D-6948-A98E-236D5ECBC3FF}" name="t2cu" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{D6E44FEE-839E-8D45-BE21-BF61FDD7208F}" name="SKIP" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2576E5F3-F6FB-A148-88F9-7DE51827E244}" name="Table7" displayName="Table7" ref="A1:E4" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="A1:E4" xr:uid="{53489C08-B6AB-264E-AD35-1FF7F63D170E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2694,19 +2727,19 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="33"/>
-    <tableColumn id="1" xr3:uid="{0624CFA4-F6C8-D846-9648-BFA84E5E19BD}" name="SKIP" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{9F00E9D8-F9CB-714B-8445-E26440DB3957}" name="tradingPartner" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{50F81C84-FE38-A44D-A41E-61752D4C3DC4}" name="createdBy" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{043C2551-D34E-364E-8939-D3F2091FAD79}" name="selectorTotal" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{8F70CAE4-FFF8-DC45-9394-34D962370E61}" name="selectorNum" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{0624CFA4-F6C8-D846-9648-BFA84E5E19BD}" name="SKIP" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:H5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A1:H5" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9BD48658-655E-0C4A-B975-66787BC4D4B6}" name="Table10" displayName="Table10" ref="A1:I5" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="A1:I5" xr:uid="{00C24615-0CEB-BA46-9A0D-2DF5F28DFD3C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2715,15 +2748,17 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="Trading Partner" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="SCAC" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{A1748E27-D6A4-EE42-86D0-6C6739CDB0DC}" name="BTC" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6F092B60-79E4-164F-BD1C-798DCF2D379B}" name="Corp Acct" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{D4701DF2-1CFF-7147-9AE0-075DE4FC5844}" name="BU" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{40A4A830-9458-204F-B09B-879E27281E1A}" name="SO" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{F56EDCFC-C0D1-BA47-A3C6-E646104EFFC4}" name="Fleet" dataDxfId="20"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{85030897-D1E7-2C43-974D-6C721A342EBB}" name="Trading Partner" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{BBEC5B11-0741-8D44-8E5D-01804D7A4C02}" name="SCAC" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{A1748E27-D6A4-EE42-86D0-6C6739CDB0DC}" name="BTC" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{6F092B60-79E4-164F-BD1C-798DCF2D379B}" name="Corp Acct" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{D4701DF2-1CFF-7147-9AE0-075DE4FC5844}" name="BU" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{40A4A830-9458-204F-B09B-879E27281E1A}" name="SO" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{F56EDCFC-C0D1-BA47-A3C6-E646104EFFC4}" name="Fleet" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{7F763B2A-94F1-EE4C-9917-7D009800ABD6}" name="Convert" dataDxfId="20"/>
     <tableColumn id="8" xr3:uid="{6CC83267-4862-7D4E-9AD1-52EF248B010A}" name="SKIP" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -3068,7 +3103,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3121,19 +3156,21 @@
       <c r="F2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="9">
-        <v>3</v>
-      </c>
+      <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
     </row>
   </sheetData>
@@ -3153,7 +3190,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3242,9 +3279,7 @@
       <c r="L2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3275,7 +3310,9 @@
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
+      <c r="M3" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -3388,9 +3425,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3399,7 +3434,9 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -3425,20 +3462,20 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="3"/>
-    <col min="2" max="8" width="9.6640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="18.1640625" style="3"/>
+    <col min="2" max="9" width="9.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="18.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -3461,14 +3498,17 @@
         <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="16"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>53</v>
       </c>
@@ -3485,12 +3525,15 @@
       <c r="H2" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="17"/>
+      <c r="I2" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>53</v>
       </c>
@@ -3505,12 +3548,15 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
@@ -3527,8 +3573,9 @@
       <c r="H4" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>44</v>
       </c>
@@ -3542,7 +3589,8 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="10" t="b">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>